<commit_message>
DB Schema and Initial Dump
</commit_message>
<xml_diff>
--- a/documentations/SRS Chap 2 Outline.xlsx
+++ b/documentations/SRS Chap 2 Outline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Process" sheetId="2" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>create_special_account</t>
-  </si>
-  <si>
     <t xml:space="preserve">PM </t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>views financial records</t>
+  </si>
+  <si>
+    <t>register</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -442,73 +442,73 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,13 +529,13 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -565,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>